<commit_message>
contact and forgot password page updates
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ContactPage Jonnie.xlsx
+++ b/Testing Spreadsheet v1.0 ContactPage Jonnie.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -21,7 +26,7 @@
   <definedNames>
     <definedName name="_Toc407532261" localSheetId="0">Reqs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -31,7 +36,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +74,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="241">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -1386,7 +1391,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1408,7 +1413,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1421,7 +1425,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1434,7 +1437,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1512,7 +1514,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1530,7 +1531,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1609,11 +1610,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53743616"/>
-        <c:axId val="53745152"/>
+        <c:axId val="-274812496"/>
+        <c:axId val="-274806512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53743616"/>
+        <c:axId val="-274812496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53745152"/>
+        <c:crossAx val="-274806512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1631,7 +1632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53745152"/>
+        <c:axId val="-274806512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53743616"/>
+        <c:crossAx val="-274812496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1809,7 +1810,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1844,7 +1845,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2092,8 +2093,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2261,7 @@
         <v>140</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2274,7 +2275,7 @@
         <v>143</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2316,7 +2317,7 @@
         <v>143</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2329,7 +2330,9 @@
       <c r="C15" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2341,7 +2344,9 @@
       <c r="C16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -2353,7 +2358,9 @@
       <c r="C17" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2365,7 +2372,9 @@
       <c r="C18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2373,7 +2382,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
@@ -2388,15 +2397,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]Settings!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D15:D18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>[2]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D14</xm:sqref>
+          <xm:sqref>D6:D18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2411,8 +2414,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I23"/>
+    <sheetView topLeftCell="B18" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,8 +2896,12 @@
       <c r="D10" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G10" s="12">
         <v>42108</v>
       </c>
@@ -2932,8 +2939,12 @@
       <c r="D11" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="12">
         <v>42108</v>
       </c>
@@ -2964,8 +2975,12 @@
       <c r="D12" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G12" s="12">
         <v>42108</v>
       </c>
@@ -2996,8 +3011,12 @@
       <c r="D13" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G13" s="12">
         <v>42108</v>
       </c>
@@ -3028,8 +3047,12 @@
       <c r="D14" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="G14" s="12">
         <v>42108</v>
       </c>
@@ -3060,8 +3083,12 @@
       <c r="D15" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G15" s="12">
         <v>42108</v>
       </c>
@@ -3092,8 +3119,12 @@
       <c r="D16" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G16" s="12">
         <v>42108</v>
       </c>
@@ -3124,8 +3155,12 @@
       <c r="D17" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G17" s="12">
         <v>42108</v>
       </c>
@@ -3156,8 +3191,12 @@
       <c r="D18" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G18" s="12">
         <v>42108</v>
       </c>
@@ -3188,8 +3227,12 @@
       <c r="D19" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G19" s="12">
         <v>42108</v>
       </c>
@@ -3220,8 +3263,12 @@
       <c r="D20" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G20" s="12">
         <v>42108</v>
       </c>
@@ -3252,8 +3299,12 @@
       <c r="D21" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G21" s="12">
         <v>42108</v>
       </c>
@@ -3284,8 +3335,12 @@
       <c r="D22" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+      <c r="E22" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G22" s="12">
         <v>42108</v>
       </c>
@@ -3316,8 +3371,12 @@
       <c r="D23" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G23" s="12">
         <v>42108</v>
       </c>
@@ -5328,7 +5387,7 @@
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8 F24:F159</xm:sqref>
+          <xm:sqref>F2:F8 F24:F159 F13:F22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -5358,13 +5417,13 @@
           <x14:formula1>
             <xm:f>[1]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F10:F23</xm:sqref>
+          <xm:sqref>H10:H23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>H10:H23</xm:sqref>
+          <xm:sqref>F10:F12 F23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5379,7 +5438,7 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -6025,12 +6084,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -6144,6 +6197,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
@@ -6153,15 +6212,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6175,4 +6225,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>